<commit_message>
Observações no excel Regras de negócio - Revisão
</commit_message>
<xml_diff>
--- a/TCC_ParteComum/Regras de negócio - Revisão.xlsx
+++ b/TCC_ParteComum/Regras de negócio - Revisão.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
   <si>
     <t>Se a solicitação de agendamento não puder ser atendida, o paciente é informado e o processo encerrado.</t>
   </si>
@@ -498,12 +498,21 @@
       <t>São regras excluídas, lembro que o Takai disse que não precisaríamos renumerá-las. Mantemos assim ou alteramos?</t>
     </r>
   </si>
+  <si>
+    <t>Alexandre: Falamos da RN-0031? Se for ela, sugiro a exclusão, visto que essa regra se adequa mais a um requisito de sistema.</t>
+  </si>
+  <si>
+    <t>Alexandre: Concordo Tati: "e na maioria das vezes (Falando em mundo real) as razões sociais - nome - podem ser iguais, mas com CNPJ diferentes."</t>
+  </si>
+  <si>
+    <t>Alexandre: Pessoal, dá uma olhada na sugestão abaixo. Quando estava montando o processo de Palestra, cujo processo de agendamento é igual ao de consulta e avaliação, notei que pode ter alguma inconsistência.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -547,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -563,6 +572,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,10 +595,521 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3657600" cy="5410201"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CaixaDeTexto 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8639175" y="19659599"/>
+          <a:ext cx="3657600" cy="5410201"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="3175">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Reagendar Palestra (como está)</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="900">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1 - Recepcionista recebe solicitação de reagendamento de palestra;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         RN-0034: A empresa deve solicitar o reagendamento da palestra com 24 horas de antecedência, a solicitação é atendida e o processo é encerrado.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>2 – Recepcionista verifica o agendamento da empresa;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>3- Recepcionista verifica agenda e informa à empresa os horários disponíveis;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         RN-0035: Se a solicitação de reagendamento não puder ser atendida, a empresa é informada e o processo encerrado.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>4 – Recepcionista realiza o reagendamento da palestra;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         RN-0036: Se a empresa solicitar o reagendamento da palestra depois do prazo de 24hrs de antecedência, será gerada uma cobrança conforme previsto em contrato e o processo é encerrado.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>       </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>5 - Recepcionista realiza o retorno da solicitação de reagendamento;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>6 – O processo é encerrado.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="900" b="1" i="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="900" b="1" i="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900" b="1" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Reagendar Palestra (sugestão de mudança)</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="900">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1 - Recepcionista recebe solicitação de reagendamento de palestra;</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="900">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="900">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>2 – Recepcionista verifica o agendamento da empresa;</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="900">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900" i="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>RN-0036: Se a empresa solicitar o reagendamento com menos de 24 horas de antecedência, é informada de que será gerada uma cobrança conforme previsto em contrato. Caso a empresa desista da solicitação de reagendamento, o processo é encerrado.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>3- Recepcionista verifica agenda e informa à empresa os horários disponíveis;</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="900">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         RN-0035: Se a solicitação de reagendamento não puder ser atendida, a empresa é informada e o processo encerrado.</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="900">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>4 – Recepcionista realiza o reagendamento da palestra;</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="900">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                </a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="900">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>5 - Recepcionista realiza o retorno da solicitação de reagendamento;</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="900">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="900">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="900" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>6 – O processo é encerrado.</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="900">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -621,9 +1147,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -655,27 +1181,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -707,27 +1215,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -900,23 +1390,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="120.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="29.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -930,7 +1421,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -938,7 +1429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -946,7 +1437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="75">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -960,7 +1451,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="30">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -968,7 +1459,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -976,7 +1467,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="60">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -990,7 +1481,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -998,7 +1489,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="60">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1012,7 +1503,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1020,7 +1511,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1029,7 +1520,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1038,7 +1529,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1046,7 +1537,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="60">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1060,7 +1551,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1068,7 +1559,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="105">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1082,7 +1573,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1090,7 +1581,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1098,7 +1589,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="60">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1112,7 +1603,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1120,7 +1611,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="60">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1134,7 +1625,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="60">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1148,27 +1639,27 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1176,7 +1667,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1184,7 +1675,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1192,7 +1683,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1200,7 +1691,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="105">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1213,8 +1704,11 @@
       <c r="D31" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="E31" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="165">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1227,8 +1721,11 @@
       <c r="D32" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="E32" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="165">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1242,27 +1739,33 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="75">
       <c r="B35" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="120">
+      <c r="C37" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1270,12 +1773,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>